<commit_message>
updated pom.xml remove log4j
</commit_message>
<xml_diff>
--- a/src/test/java/SayaliAssignment/guru99creds.xlsx
+++ b/src/test/java/SayaliAssignment/guru99creds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPA Base\Projects\firstauto\src\test\java\SayaliAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403A5480-55A2-4FDC-A6CC-7A97D0D63BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C51A36-F084-4C69-A164-F132EF5997D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A98472FE-F696-4AC2-A290-A8CA5831A575}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>ezAbezu</t>
+  </si>
+  <si>
+    <t>rreterheh3</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -486,15 +489,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D0DAD-1343-4480-8758-1BB4F63F2D2C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>